<commit_message>
Lecteur Fichier needs work
</commit_message>
<xml_diff>
--- a/MV_offres_de_reservation.xlsx
+++ b/MV_offres_de_reservation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0.sharepoint.com/sites/LOG2400-quipedesenseignants/Shared Documents/General/travauxPratiques/A2024/TP4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alons\Documents\POLYTECHNIQUE\TRAVAIL EQUIPE\2400\LOG2400_TP4-5_2291747\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="11_D769545181EB47DABAAC04DD3F6FB52AC9E24922" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13EE7893-EE4A-4C11-B569-F2008C16000D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FE1CF1-8747-4196-8C6F-505C860499C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="15576" windowHeight="11784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vols" sheetId="1" r:id="rId1"/>
@@ -807,25 +807,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="4" max="5" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -913,7 +912,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -957,7 +956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1001,7 +1000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1045,7 +1044,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>143</v>
       </c>
@@ -1089,7 +1088,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1133,7 +1132,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1177,7 +1176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1265,7 +1264,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1353,7 +1352,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -1397,7 +1396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -1441,7 +1440,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -1497,18 +1496,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5960AAA9-12EE-4C65-ADDB-C727DA391653}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1548,7 +1547,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -1568,7 +1567,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1588,7 +1587,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>93</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>106</v>
       </c>
@@ -1628,7 +1627,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>108</v>
       </c>
@@ -1648,7 +1647,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>110</v>
       </c>
@@ -1668,7 +1667,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>112</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -1708,7 +1707,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>118</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>121</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>124</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>127</v>
       </c>
@@ -1788,7 +1787,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>130</v>
       </c>
@@ -1817,17 +1816,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B6B216-54EC-4C57-824D-642CA25FD9D9}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="77.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1861,7 +1860,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1878,7 +1877,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1895,7 +1894,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>83</v>
       </c>
@@ -1912,7 +1911,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1929,7 +1928,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>133</v>
       </c>
@@ -1946,7 +1945,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>134</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>135</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>136</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>137</v>
       </c>
@@ -2014,7 +2013,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>138</v>
       </c>
@@ -2031,7 +2030,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>139</v>
       </c>
@@ -2048,7 +2047,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>140</v>
       </c>
@@ -2065,7 +2064,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>141</v>
       </c>
@@ -2082,7 +2081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>142</v>
       </c>
@@ -2105,15 +2104,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2d78f529-18b9-49f0-a517-5cc9110fa36b">
@@ -2122,6 +2112,15 @@
     <TaxCatchAll xmlns="913bbb79-a9c0-46f0-9840-73e385eae5c9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2326,14 +2325,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB11196B-6C77-43B0-A109-2A0D59E852E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{292943AC-3FF1-4000-B94B-7262E0EAFFFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2350,6 +2341,29 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB11196B-6C77-43B0-A109-2A0D59E852E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547CB307-FD58-4443-A76D-B01C62CE0428}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547CB307-FD58-4443-A76D-B01C62CE0428}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2d78f529-18b9-49f0-a517-5cc9110fa36b"/>
+    <ds:schemaRef ds:uri="913bbb79-a9c0-46f0-9840-73e385eae5c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>